<commit_message>
- Added library wandb for online logging of metrics - Added possibility to turn off progress bars - Fixed some minor issues
</commit_message>
<xml_diff>
--- a/results_for_thesis/Experiment_results.xlsx
+++ b/results_for_thesis/Experiment_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\Masterarbeit\Software\Ensemble_Embedding_for_Link_Prediction\results_for_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D94C85-E9F0-47EE-8DC3-3E82DEF297C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DF432E-0D6E-4293-8AC7-B993087439A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{BC009FAC-19B4-41D4-83AF-8F1B5375A1FF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{BC009FAC-19B4-41D4-83AF-8F1B5375A1FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
   <si>
     <t>Hyperparameters</t>
   </si>
@@ -162,16 +162,48 @@
   </si>
   <si>
     <t>Comparison theta</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>N10</t>
+  </si>
+  <si>
+    <t>rank_deviation</t>
+  </si>
+  <si>
+    <t>HITS@10</t>
+  </si>
+  <si>
+    <t>HITS@3</t>
+  </si>
+  <si>
+    <t>HITS@1</t>
+  </si>
+  <si>
+    <t>MRR</t>
+  </si>
+  <si>
+    <t>epochs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -227,26 +259,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,26 +613,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF38"/>
+  <dimension ref="A1:AF42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U50" sqref="U50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
@@ -609,7 +640,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -620,40 +651,40 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M3" s="3"/>
@@ -685,116 +716,102 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="4">
         <v>200</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>32</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <v>0.1</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="4">
         <v>5</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="O5" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5">
         <v>199</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5">
         <v>6018.35</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5">
         <v>0.40699999999999997</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5">
         <v>0.38800000000000001</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5">
         <v>0.41399999999999998</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5">
         <v>0.443</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5">
         <v>0.70606500000000005</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
       <c r="M6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4" t="s">
+      <c r="O6" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6">
         <v>199</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6">
         <v>6018.35</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6">
         <v>0.40699999999999997</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6">
         <v>0.38800000000000001</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6">
         <v>0.41399999999999998</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6">
         <v>0.443</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6">
         <v>0.70606500000000005</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W6">
         <v>0</v>
       </c>
       <c r="Z6" t="s">
@@ -802,60 +819,47 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4" t="s">
+      <c r="O7" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7">
         <v>199</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7">
         <v>6049.17</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7">
         <v>0.40400000000000003</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T7" s="4">
+      <c r="T7">
         <v>0.41299999999999998</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7">
         <v>0.44400000000000001</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7">
         <v>0.70455699999999999</v>
       </c>
-      <c r="W7" s="4">
+      <c r="W7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
       <c r="M8" s="3"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -890,239 +894,212 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="Y9" s="5"/>
+      <c r="Y9" s="4"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="4">
         <v>50</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>32</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>0.1</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="4">
         <v>5</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="4">
         <v>5</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4" t="s">
+      <c r="O10" t="s">
         <v>25</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10">
         <v>24</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10">
         <v>11054.3837890625</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10">
         <v>0.33007094264030401</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10">
         <v>0.28707975149154602</v>
       </c>
-      <c r="T10" s="4">
+      <c r="T10">
         <v>0.36025047302245999</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10">
         <v>0.40013182163238498</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10">
         <v>0.46006000041961598</v>
       </c>
-      <c r="W10" s="4">
+      <c r="W10">
         <v>2</v>
       </c>
-      <c r="Y10" s="7" t="s">
+      <c r="Y10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Z10" s="4">
+      <c r="Z10">
         <v>11054.3837890625</v>
       </c>
-      <c r="AA10" s="4">
+      <c r="AA10">
         <v>0.33007094264030401</v>
       </c>
-      <c r="AB10" s="4">
+      <c r="AB10">
         <v>0.28707975149154602</v>
       </c>
-      <c r="AC10" s="4">
+      <c r="AC10">
         <v>0.36025047302245999</v>
       </c>
-      <c r="AD10" s="4">
+      <c r="AD10">
         <v>0.40013182163238498</v>
       </c>
-      <c r="AE10" s="4">
+      <c r="AE10">
         <v>0.46006000041961598</v>
       </c>
-      <c r="AF10" s="4">
+      <c r="AF10">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4" t="s">
+      <c r="O11" t="s">
         <v>31</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11">
         <v>49</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11">
         <v>11349.9462890625</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11">
         <v>0.327791988849639</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11">
         <v>0.28444296121597201</v>
       </c>
-      <c r="T11" s="4">
+      <c r="T11">
         <v>0.35794329643249501</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11">
         <v>0.39980223774909901</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V11">
         <v>0.44562217593192999</v>
       </c>
-      <c r="W11" s="4">
+      <c r="W11">
         <v>1</v>
       </c>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="4">
+      <c r="Y11" s="4"/>
+      <c r="Z11">
         <v>11349.9462890625</v>
       </c>
-      <c r="AA11" s="4">
+      <c r="AA11">
         <v>0.327791988849639</v>
       </c>
-      <c r="AB11" s="4">
+      <c r="AB11">
         <v>0.28444296121597201</v>
       </c>
-      <c r="AC11" s="4">
+      <c r="AC11">
         <v>0.35794329643249501</v>
       </c>
-      <c r="AD11" s="4">
+      <c r="AD11">
         <v>0.39980223774909901</v>
       </c>
-      <c r="AE11" s="4">
+      <c r="AE11">
         <v>0.44562217593192999</v>
       </c>
-      <c r="AF11" s="4">
+      <c r="AF11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4" t="s">
+      <c r="O12" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12">
         <v>49</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12">
         <v>10579.748535156201</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12">
         <v>0.32429946959018702</v>
       </c>
-      <c r="S12" s="4">
+      <c r="S12">
         <v>0.277440965175628</v>
       </c>
-      <c r="T12" s="4">
+      <c r="T12">
         <v>0.35880663990974399</v>
       </c>
-      <c r="U12" s="4">
+      <c r="U12">
         <v>0.39996808767318698</v>
       </c>
-      <c r="V12" s="4">
+      <c r="V12">
         <v>0.48324504494666998</v>
       </c>
-      <c r="W12" s="4">
+      <c r="W12">
         <v>1</v>
       </c>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="4">
+      <c r="Y12" s="4"/>
+      <c r="Z12">
         <v>10579.748535156201</v>
       </c>
-      <c r="AA12" s="4">
+      <c r="AA12">
         <v>0.32429946959018702</v>
       </c>
-      <c r="AB12" s="4">
+      <c r="AB12">
         <v>0.277440965175628</v>
       </c>
-      <c r="AC12" s="4">
+      <c r="AC12">
         <v>0.35880663990974399</v>
       </c>
-      <c r="AD12" s="4">
+      <c r="AD12">
         <v>0.39996808767318698</v>
       </c>
-      <c r="AE12" s="4">
+      <c r="AE12">
         <v>0.48324504494666998</v>
       </c>
-      <c r="AF12" s="4">
+      <c r="AF12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
       <c r="M13" s="3"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1134,7 +1111,7 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="Y13" s="6"/>
+      <c r="Y13" s="5"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
@@ -1144,239 +1121,212 @@
       <c r="AF13" s="2"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="Y14" s="5"/>
+      <c r="Y14" s="4"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="4">
         <v>50</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="4">
         <v>32</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="4">
         <v>0.1</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="4">
         <v>5</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="4">
         <v>5</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4" t="s">
+      <c r="O15" t="s">
         <v>25</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15">
         <v>24</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15">
         <v>10199.530761718701</v>
       </c>
-      <c r="R15" s="4">
+      <c r="R15">
         <v>0.32315351068973502</v>
       </c>
-      <c r="S15" s="4">
+      <c r="S15">
         <v>0.27982860803604098</v>
       </c>
-      <c r="T15" s="4">
+      <c r="T15">
         <v>0.35415291786193798</v>
       </c>
-      <c r="U15" s="4">
+      <c r="U15">
         <v>0.39255106449127197</v>
       </c>
-      <c r="V15" s="4">
+      <c r="V15">
         <v>0.50181806087493896</v>
       </c>
-      <c r="W15" s="4">
+      <c r="W15">
         <v>5</v>
       </c>
-      <c r="Y15" s="7" t="s">
+      <c r="Y15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Z15" s="4">
+      <c r="Z15">
         <v>10199.530761718701</v>
       </c>
-      <c r="AA15" s="4">
+      <c r="AA15">
         <v>0.32315351068973502</v>
       </c>
-      <c r="AB15" s="4">
+      <c r="AB15">
         <v>0.27982860803604098</v>
       </c>
-      <c r="AC15" s="4">
+      <c r="AC15">
         <v>0.35415291786193798</v>
       </c>
-      <c r="AD15" s="4">
+      <c r="AD15">
         <v>0.39255106449127197</v>
       </c>
-      <c r="AE15" s="4">
+      <c r="AE15">
         <v>0.50181806087493896</v>
       </c>
-      <c r="AF15" s="4">
+      <c r="AF15">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4" t="s">
+      <c r="O16" t="s">
         <v>31</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16">
         <v>49</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16">
         <v>10711.874511718701</v>
       </c>
-      <c r="R16" s="4">
+      <c r="R16">
         <v>0.32263678312301602</v>
       </c>
-      <c r="S16" s="4">
+      <c r="S16">
         <v>0.27818059921264598</v>
       </c>
-      <c r="T16" s="4">
+      <c r="T16">
         <v>0.35629531741142201</v>
       </c>
-      <c r="U16" s="4">
+      <c r="U16">
         <v>0.39370468258857699</v>
       </c>
-      <c r="V16" s="4">
+      <c r="V16">
         <v>0.47679090499877902</v>
       </c>
-      <c r="W16" s="4">
+      <c r="W16">
         <v>2</v>
       </c>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="4">
+      <c r="Y16" s="4"/>
+      <c r="Z16">
         <v>10711.874511718701</v>
       </c>
-      <c r="AA16" s="4">
+      <c r="AA16">
         <v>0.32263678312301602</v>
       </c>
-      <c r="AB16" s="4">
+      <c r="AB16">
         <v>0.27818059921264598</v>
       </c>
-      <c r="AC16" s="4">
+      <c r="AC16">
         <v>0.35629531741142201</v>
       </c>
-      <c r="AD16" s="4">
+      <c r="AD16">
         <v>0.39370468258857699</v>
       </c>
-      <c r="AE16" s="4">
+      <c r="AE16">
         <v>0.47679090499877902</v>
       </c>
-      <c r="AF16" s="4">
+      <c r="AF16">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4" t="s">
+      <c r="O17" t="s">
         <v>30</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17">
         <v>49</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="Q17">
         <v>10022.305175781201</v>
       </c>
-      <c r="R17" s="4">
+      <c r="R17">
         <v>0.320089802145957</v>
       </c>
-      <c r="S17" s="4">
+      <c r="S17">
         <v>0.276005119085311</v>
       </c>
-      <c r="T17" s="4">
+      <c r="T17">
         <v>0.35003191232681202</v>
       </c>
-      <c r="U17" s="4">
+      <c r="U17">
         <v>0.393746018409729</v>
       </c>
-      <c r="V17" s="4">
+      <c r="V17">
         <v>0.51047521829605103</v>
       </c>
-      <c r="W17" s="4">
+      <c r="W17">
         <v>2</v>
       </c>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="4">
+      <c r="Y17" s="4"/>
+      <c r="Z17">
         <v>10022.305175781201</v>
       </c>
-      <c r="AA17" s="4">
+      <c r="AA17">
         <v>0.320089802145957</v>
       </c>
-      <c r="AB17" s="4">
+      <c r="AB17">
         <v>0.276005119085311</v>
       </c>
-      <c r="AC17" s="4">
+      <c r="AC17">
         <v>0.35003191232681202</v>
       </c>
-      <c r="AD17" s="4">
+      <c r="AD17">
         <v>0.393746018409729</v>
       </c>
-      <c r="AE17" s="4">
+      <c r="AE17">
         <v>0.51047521829605103</v>
       </c>
-      <c r="AF17" s="4">
+      <c r="AF17">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
       <c r="M18" s="3"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1388,7 +1338,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-      <c r="Y18" s="6"/>
+      <c r="Y18" s="5"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
@@ -1398,238 +1348,211 @@
       <c r="AF18" s="2"/>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="Y19" s="5"/>
+      <c r="Y19" s="4"/>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="4">
         <v>50</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>32</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="4">
         <v>0.1</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="4">
         <v>5</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="4">
         <v>5</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="L20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4" t="s">
+      <c r="O20" t="s">
         <v>25</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20">
         <v>34</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="Q20">
         <v>11216.779785156201</v>
       </c>
-      <c r="R20" s="4">
+      <c r="R20">
         <v>0.31828357279300601</v>
       </c>
-      <c r="S20" s="4">
+      <c r="S20">
         <v>0.27719181776046697</v>
       </c>
-      <c r="T20" s="4">
+      <c r="T20">
         <v>0.34838497638702298</v>
       </c>
-      <c r="U20" s="4">
+      <c r="U20">
         <v>0.38546472787857</v>
       </c>
-      <c r="V20" s="4">
+      <c r="V20">
         <v>0.45212706923484802</v>
       </c>
-      <c r="W20" s="4">
+      <c r="W20">
         <v>3</v>
       </c>
-      <c r="Y20" s="7" t="s">
+      <c r="Y20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Z20" s="4">
+      <c r="Z20">
         <v>11216.779785156201</v>
       </c>
-      <c r="AA20" s="4">
+      <c r="AA20">
         <v>0.31828357279300601</v>
       </c>
-      <c r="AB20" s="4">
+      <c r="AB20">
         <v>0.27719181776046697</v>
       </c>
-      <c r="AC20" s="4">
+      <c r="AC20">
         <v>0.34838497638702298</v>
       </c>
-      <c r="AD20" s="4">
+      <c r="AD20">
         <v>0.38546472787857</v>
       </c>
-      <c r="AE20" s="4">
+      <c r="AE20">
         <v>0.45212706923484802</v>
       </c>
-      <c r="AF20" s="4">
+      <c r="AF20">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4" t="s">
+      <c r="O21" t="s">
         <v>31</v>
       </c>
-      <c r="P21" s="4">
+      <c r="P21">
         <v>49</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="Q21">
         <v>10983.547363281201</v>
       </c>
-      <c r="R21" s="4">
+      <c r="R21">
         <v>0.31679619848728102</v>
       </c>
-      <c r="S21" s="4">
+      <c r="S21">
         <v>0.275049448013305</v>
       </c>
-      <c r="T21" s="4">
+      <c r="T21">
         <v>0.34640738368034302</v>
       </c>
-      <c r="U21" s="4">
+      <c r="U21">
         <v>0.38414633274078303</v>
       </c>
-      <c r="V21" s="4">
+      <c r="V21">
         <v>0.46352019906044001</v>
       </c>
-      <c r="W21" s="4">
+      <c r="W21">
         <v>2</v>
       </c>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="4">
+      <c r="Y21" s="4"/>
+      <c r="Z21">
         <v>10983.547363281201</v>
       </c>
-      <c r="AA21" s="4">
+      <c r="AA21">
         <v>0.31679619848728102</v>
       </c>
-      <c r="AB21" s="4">
+      <c r="AB21">
         <v>0.275049448013305</v>
       </c>
-      <c r="AC21" s="4">
+      <c r="AC21">
         <v>0.34640738368034302</v>
       </c>
-      <c r="AD21" s="4">
+      <c r="AD21">
         <v>0.38414633274078303</v>
       </c>
-      <c r="AE21" s="4">
+      <c r="AE21">
         <v>0.46352019906044001</v>
       </c>
-      <c r="AF21" s="4">
+      <c r="AF21">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4" t="s">
+      <c r="O22" t="s">
         <v>30</v>
       </c>
-      <c r="P22" s="4">
+      <c r="P22">
         <v>49</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="Q22">
         <v>10969.7890625</v>
       </c>
-      <c r="R22" s="4">
+      <c r="R22">
         <v>0.31487408280372597</v>
       </c>
-      <c r="S22" s="4">
+      <c r="S22">
         <v>0.27089980244636502</v>
       </c>
-      <c r="T22" s="4">
+      <c r="T22">
         <v>0.34636247158050498</v>
       </c>
-      <c r="U22" s="4">
+      <c r="U22">
         <v>0.38513082265853799</v>
       </c>
-      <c r="V22" s="4">
+      <c r="V22">
         <v>0.46419218182563698</v>
       </c>
-      <c r="W22" s="4">
+      <c r="W22">
         <v>4</v>
       </c>
-      <c r="Z22" s="4">
+      <c r="Z22">
         <v>10969.7890625</v>
       </c>
-      <c r="AA22" s="4">
+      <c r="AA22">
         <v>0.31487408280372597</v>
       </c>
-      <c r="AB22" s="4">
+      <c r="AB22">
         <v>0.27089980244636502</v>
       </c>
-      <c r="AC22" s="4">
+      <c r="AC22">
         <v>0.34636247158050498</v>
       </c>
-      <c r="AD22" s="4">
+      <c r="AD22">
         <v>0.38513082265853799</v>
       </c>
-      <c r="AE22" s="4">
+      <c r="AE22">
         <v>0.46419218182563698</v>
       </c>
-      <c r="AF22" s="4">
+      <c r="AF22">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
       <c r="M23" s="3"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1643,168 +1566,141 @@
       <c r="W23" s="2"/>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="4">
         <v>50</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="4">
         <v>32</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="4">
         <v>0.1</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="4">
         <v>10</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="4">
         <v>5</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L25" s="7" t="s">
+      <c r="L25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4" t="s">
+      <c r="O25" t="s">
         <v>25</v>
       </c>
-      <c r="P25" s="4">
+      <c r="P25">
         <v>49</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="Q25">
         <v>10413.304199218701</v>
       </c>
-      <c r="R25" s="4">
+      <c r="R25">
         <v>0.36210517585277502</v>
       </c>
-      <c r="S25" s="4">
+      <c r="S25">
         <v>0.33256429433822599</v>
       </c>
-      <c r="T25" s="4">
+      <c r="T25">
         <v>0.37821358442306502</v>
       </c>
-      <c r="U25" s="4">
+      <c r="U25">
         <v>0.41282135248184199</v>
       </c>
-      <c r="V25" s="4">
+      <c r="V25">
         <v>0.49137559533119202</v>
       </c>
-      <c r="W25" s="4">
+      <c r="W25">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4" t="s">
+      <c r="O26" t="s">
         <v>31</v>
       </c>
-      <c r="P26" s="4">
+      <c r="P26">
         <v>49</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="Q26">
         <v>10413.304199218701</v>
       </c>
-      <c r="R26" s="4">
+      <c r="R26">
         <v>0.36210517585277502</v>
       </c>
-      <c r="S26" s="4">
+      <c r="S26">
         <v>0.33256429433822599</v>
       </c>
-      <c r="T26" s="4">
+      <c r="T26">
         <v>0.37821358442306502</v>
       </c>
-      <c r="U26" s="4">
+      <c r="U26">
         <v>0.41282135248184199</v>
       </c>
-      <c r="V26" s="4">
+      <c r="V26">
         <v>0.49137559533119202</v>
       </c>
-      <c r="W26" s="4">
+      <c r="W26">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4" t="s">
+      <c r="O27" t="s">
         <v>30</v>
       </c>
-      <c r="P27" s="4">
+      <c r="P27">
         <v>49</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="Q27">
         <v>10512.7177734375</v>
       </c>
-      <c r="R27" s="4">
+      <c r="R27">
         <v>0.35090760886669098</v>
       </c>
-      <c r="S27" s="4">
+      <c r="S27">
         <v>0.32195276021957397</v>
       </c>
-      <c r="T27" s="4">
+      <c r="T27">
         <v>0.367581367492675</v>
       </c>
-      <c r="U27" s="4">
+      <c r="U27">
         <v>0.40220165252685502</v>
       </c>
-      <c r="V27" s="4">
+      <c r="V27">
         <v>0.48651939630508401</v>
       </c>
-      <c r="W27" s="4">
+      <c r="W27">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
       <c r="M28" s="3"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -1818,168 +1714,141 @@
       <c r="W28" s="2"/>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="4">
         <v>50</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="4">
         <v>32</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="4">
         <v>0.1</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="4">
         <v>30</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="4">
         <v>5</v>
       </c>
-      <c r="K30" s="7" t="s">
+      <c r="K30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L30" s="7" t="s">
+      <c r="L30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4" t="s">
+      <c r="O30" t="s">
         <v>25</v>
       </c>
-      <c r="P30" s="4">
+      <c r="P30">
         <v>14</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="Q30">
         <v>10784.425292968701</v>
       </c>
-      <c r="R30" s="4">
+      <c r="R30">
         <v>0.40130004286766002</v>
       </c>
-      <c r="S30" s="4">
+      <c r="S30">
         <v>0.37063282728195102</v>
       </c>
-      <c r="T30" s="4">
+      <c r="T30">
         <v>0.414634138345718</v>
       </c>
-      <c r="U30" s="4">
+      <c r="U30">
         <v>0.46077784895896901</v>
       </c>
-      <c r="V30" s="4">
+      <c r="V30">
         <v>0.47324687242507901</v>
       </c>
-      <c r="W30" s="4">
+      <c r="W30">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4" t="s">
+      <c r="O31" t="s">
         <v>31</v>
       </c>
-      <c r="P31" s="4">
+      <c r="P31">
         <v>49</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="Q31">
         <v>11988.481933593701</v>
       </c>
-      <c r="R31" s="4">
+      <c r="R31">
         <v>0.37767584621906197</v>
       </c>
-      <c r="S31" s="4">
+      <c r="S31">
         <v>0.35085695981979298</v>
       </c>
-      <c r="T31" s="4">
+      <c r="T31">
         <v>0.38892552256584101</v>
       </c>
-      <c r="U31" s="4">
+      <c r="U31">
         <v>0.43029004335403398</v>
       </c>
-      <c r="V31" s="4">
+      <c r="V31">
         <v>0.41443073749542197</v>
       </c>
-      <c r="W31" s="4">
+      <c r="W31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4" t="s">
+      <c r="O32" t="s">
         <v>30</v>
       </c>
-      <c r="P32" s="4">
+      <c r="P32">
         <v>49</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="Q32">
         <v>10624.279296875</v>
       </c>
-      <c r="R32" s="4">
+      <c r="R32">
         <v>0.41044580936431801</v>
       </c>
-      <c r="S32" s="4">
+      <c r="S32">
         <v>0.37922781705856301</v>
       </c>
-      <c r="T32" s="4">
+      <c r="T32">
         <v>0.42405873537063599</v>
       </c>
-      <c r="U32" s="4">
+      <c r="U32">
         <v>0.47176134586334201</v>
       </c>
-      <c r="V32" s="4">
+      <c r="V32">
         <v>0.48106980323791498</v>
       </c>
-      <c r="W32" s="4">
+      <c r="W32">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
       <c r="M33" s="3"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -1993,168 +1862,141 @@
       <c r="W33" s="2"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="4">
         <v>20</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="4">
         <v>32</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="4">
         <v>0.1</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="4">
         <v>60</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="I35" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J35" s="7">
+      <c r="J35" s="4">
         <v>5</v>
       </c>
-      <c r="K35" s="7" t="s">
+      <c r="K35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="7" t="s">
+      <c r="L35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4" t="s">
+      <c r="O35" t="s">
         <v>25</v>
       </c>
-      <c r="P35" s="4">
+      <c r="P35">
         <v>9</v>
       </c>
-      <c r="Q35" s="4">
+      <c r="Q35">
         <v>9943.68115234375</v>
       </c>
-      <c r="R35" s="4">
+      <c r="R35">
         <v>0.43824572861194599</v>
       </c>
-      <c r="S35" s="4">
+      <c r="S35">
         <v>0.40919578075408902</v>
       </c>
-      <c r="T35" s="4">
+      <c r="T35">
         <v>0.45517468452453602</v>
       </c>
-      <c r="U35" s="4">
+      <c r="U35">
         <v>0.49307847023010198</v>
       </c>
-      <c r="V35" s="4">
+      <c r="V35">
         <v>0.51431590318679798</v>
       </c>
-      <c r="W35" s="4">
+      <c r="W35">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4" t="s">
+      <c r="O36" t="s">
         <v>31</v>
       </c>
-      <c r="P36" s="4">
+      <c r="P36">
         <v>19</v>
       </c>
-      <c r="Q36" s="4">
+      <c r="Q36">
         <v>9813.02392578125</v>
       </c>
-      <c r="R36" s="4">
+      <c r="R36">
         <v>0.42470735311508101</v>
       </c>
-      <c r="S36" s="4">
+      <c r="S36">
         <v>0.39568227529525701</v>
       </c>
-      <c r="T36" s="4">
+      <c r="T36">
         <v>0.43803560733795099</v>
       </c>
-      <c r="U36" s="4">
+      <c r="U36">
         <v>0.47956490516662598</v>
       </c>
-      <c r="V36" s="4">
+      <c r="V36">
         <v>0.52069830894470204</v>
       </c>
-      <c r="W36" s="4">
+      <c r="W36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4" t="s">
+      <c r="O37" t="s">
         <v>30</v>
       </c>
-      <c r="P37" s="4">
+      <c r="P37">
         <v>19</v>
       </c>
-      <c r="Q37" s="4">
+      <c r="Q37">
         <v>9866.6591796875</v>
       </c>
-      <c r="R37" s="4">
+      <c r="R37">
         <v>0.44116793572902602</v>
       </c>
-      <c r="S37" s="4">
+      <c r="S37">
         <v>0.41129547357559199</v>
       </c>
-      <c r="T37" s="4">
+      <c r="T37">
         <v>0.45500957965850802</v>
       </c>
-      <c r="U37" s="4">
+      <c r="U37">
         <v>0.49760690331459001</v>
       </c>
-      <c r="V37" s="4">
+      <c r="V37">
         <v>0.51807832717895497</v>
       </c>
-      <c r="W37" s="4">
+      <c r="W37">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
       <c r="M38" s="3"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -2167,9 +2009,105 @@
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
     </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>9</v>
+      </c>
+      <c r="R40" t="s">
+        <v>48</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="T40" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U40" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="V40" t="s">
+        <v>14</v>
+      </c>
+      <c r="W40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
+        <v>43</v>
+      </c>
+      <c r="P41">
+        <v>105</v>
+      </c>
+      <c r="Q41">
+        <v>5021.4931640625</v>
+      </c>
+      <c r="R41">
+        <v>0.42870718240737898</v>
+      </c>
+      <c r="S41">
+        <v>0.39683586359023998</v>
+      </c>
+      <c r="T41">
+        <v>0.44380354881286599</v>
+      </c>
+      <c r="U41">
+        <v>0.48895847797393799</v>
+      </c>
+      <c r="V41">
+        <v>0.75475692749023404</v>
+      </c>
+      <c r="W41">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="O42" t="s">
+        <v>42</v>
+      </c>
+      <c r="P42">
+        <v>200</v>
+      </c>
+      <c r="Q42">
+        <v>6018.35</v>
+      </c>
+      <c r="R42">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="S42">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="T42">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="U42">
+        <v>0.443</v>
+      </c>
+      <c r="V42">
+        <v>0.70606500000000005</v>
+      </c>
+      <c r="W42">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="Q1:Q39 Q43:Q1048576">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q44:Q1048576 Q1:Q38">
-    <cfRule type="colorScale" priority="63">
+    <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2180,8 +2118,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R39 R43:R1048576">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R44:R1048576 R1:R38">
-    <cfRule type="colorScale" priority="67">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2192,92 +2142,208 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1048576">
+  <conditionalFormatting sqref="S1:S39 S43:S1048576">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S44:S1048576 S1:S38">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:T39 T43:T1048576">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T44:T1048576 T1:T38">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U39 U43:U1048576">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1048576">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U44:U1048576 U1:U38">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:V39 V43:V1048576">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V44:V1048576 V1:V38">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W1:W39 W43:W1048576">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S44:S1048576 S1:S38">
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W44:W1048576 W1:W38">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y1:Y4 Y23:Y1048576 Z10:Z22">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T44:T1048576 T1:T38">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z1:Z4 Z23:Z1048576 AA10:AA22">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z6:Z7 AA1:AA4 AA23:AA1048576 AB10:AB22 Z9">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z8">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z10:Z22">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U44:U1048576 U1:U38">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="colorScale" priority="48">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA6:AA7 AB1:AB4 AB23:AB1048576 AC10:AC22 AA9">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2288,8 +2354,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V44:V1048576 V1:V38">
-    <cfRule type="colorScale" priority="47">
+  <conditionalFormatting sqref="AA8">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2300,56 +2376,96 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:V1048576">
+  <conditionalFormatting sqref="AA10:AA22">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB6:AB7 AC1:AC4 AC23:AC1048576 AD10:AD22 AB9">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W44:W1048576 W1:W38">
-    <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
+  <conditionalFormatting sqref="AB8">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB10:AB22">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z10:Z22">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA10:AA22">
-    <cfRule type="colorScale" priority="39">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC8">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2360,56 +2476,150 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z10:Z22">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
+  <conditionalFormatting sqref="AC10:AC22">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA10:AA22">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD8">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD10:AD22">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE8">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE10:AE22">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF8">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE10:AE22">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE10:AE22">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF10:AF22">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF10:AF22">
-    <cfRule type="colorScale" priority="27">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2420,116 +2630,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF10:AF22">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y1:Y4 Y23:Y1048576 Z10:Z22">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z1:Z4 Z23:Z1048576 AA10:AA22">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB10:AB22">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+  <conditionalFormatting sqref="Q41:Q42">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB10:AB22">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z6:Z7 AA1:AA4 AA23:AA1048576 AB10:AB22 Z9">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC10:AC22">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W41:W42">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC10:AC22">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA6:AA7 AB1:AB4 AB23:AB1048576 AC10:AC22 AA9">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD10:AD22">
-    <cfRule type="colorScale" priority="17">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R41:R42">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2540,44 +2666,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD10:AD22">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB6:AB7 AC1:AC4 AC23:AC1048576 AD10:AD22 AB9">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z8">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
+  <conditionalFormatting sqref="S41:S42">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA8">
-    <cfRule type="colorScale" priority="14">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T41:T42">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2588,32 +2690,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z8">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA8">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB8">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="U41:U42">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2624,20 +2702,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB8">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC8">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="V41:V42">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2648,91 +2714,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC8">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD8">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD8">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE8">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE8">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF8">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF8">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="U40" r:id="rId1" xr:uid="{9A2C4F2D-7A76-4B70-B37D-2162DD674754}"/>
+    <hyperlink ref="T40" r:id="rId2" xr:uid="{76026865-779E-4BCA-B028-52EAC8147C9A}"/>
+    <hyperlink ref="S40" r:id="rId3" xr:uid="{D897D26D-8C3B-4E60-BD51-E907AF08FF70}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="31" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="31" fitToHeight="0" orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>